<commit_message>
finish getting best model data + knit finalized experiemnt analysis
</commit_message>
<xml_diff>
--- a/best models/all_capture_model_stats.xlsx
+++ b/best models/all_capture_model_stats.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savannahweaver/Documents/github projects/Herpetology_2021/best models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F0978DB8-1F7A-634E-859A-CB9DB6CC4834}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F2B04DD7-F98D-5045-AB7D-CFC1B9ADDA36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_capture_model_stats" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="42" uniqueCount="34">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="49" uniqueCount="38">
   <si>
     <t>estimate</t>
   </si>
@@ -45,98 +45,111 @@
     <t>log(CEWL) ~</t>
   </si>
   <si>
-    <t>osmolality ~</t>
-  </si>
-  <si>
-    <t>hematocrit ~</t>
-  </si>
-  <si>
     <t>&lt; 0.0001</t>
   </si>
   <si>
     <t>&lt; 0.001</t>
   </si>
   <si>
-    <t>mass (g)</t>
-  </si>
-  <si>
-    <t>solar radiation at the time of capture (W/m2)</t>
-  </si>
-  <si>
-    <t>region (ventrum)</t>
-  </si>
-  <si>
-    <t>region (head)</t>
-  </si>
-  <si>
-    <t>region (dewlap)</t>
-  </si>
-  <si>
-    <t>region (mite patch)</t>
-  </si>
-  <si>
-    <t>(intercept)</t>
-  </si>
-  <si>
-    <t>temperature at the time of capture (℃)</t>
-  </si>
-  <si>
-    <t>absolute humidity at the time of capture (g/m2)</t>
-  </si>
-  <si>
-    <t>cloacal temperature at the time of measurement (℃)</t>
-  </si>
-  <si>
-    <t>region (ventrum) * mass (g)</t>
-  </si>
-  <si>
-    <t>region (head) * mass (g)</t>
-  </si>
-  <si>
-    <t>region (dewlap) * mass (g)</t>
-  </si>
-  <si>
-    <t>region (mite patch) * mass (g)</t>
-  </si>
-  <si>
-    <t>region (ventrum) * temperature at the time of capture (℃)</t>
-  </si>
-  <si>
-    <t>region (head) * temperature at the time of capture (℃)</t>
-  </si>
-  <si>
-    <t>region (dewlap) * temperature at the time of capture (℃)</t>
-  </si>
-  <si>
-    <t>region (mite patch) * temperature at the time of capture (℃)</t>
-  </si>
-  <si>
-    <t>region (ventrum) * absolute humidity at the time of capture (g/m2)</t>
-  </si>
-  <si>
-    <t>region (head) * absolute humidity at the time of capture (g/m2)</t>
-  </si>
-  <si>
-    <t>region (dewlap) * absolute humidity at the time of capture (g/m2)</t>
-  </si>
-  <si>
-    <t>region (mite patch) * absolute humidity at the time of capture (g/m2)</t>
-  </si>
-  <si>
-    <t>absolute humidity at the time of capture (g/m2) * temperature at the time of capture (℃)</t>
-  </si>
-  <si>
-    <t>sex (male)</t>
+    <t>Sex (male)</t>
+  </si>
+  <si>
+    <t>(Intercept)</t>
+  </si>
+  <si>
+    <t>Vapor pressure deficit at the time of capture (kPa) * temperature at the time of capture (℃)</t>
+  </si>
+  <si>
+    <t>Temperature at the time of capture (℃)</t>
+  </si>
+  <si>
+    <t>Vapor pressure deficit at the time of capture (kPa)</t>
+  </si>
+  <si>
+    <t>Region (ventrum)</t>
+  </si>
+  <si>
+    <t>Region (head)</t>
+  </si>
+  <si>
+    <t>Region (dewlap)</t>
+  </si>
+  <si>
+    <t>Region (mite patch)</t>
+  </si>
+  <si>
+    <t>Mass (g)</t>
+  </si>
+  <si>
+    <t>Cloacal temperature at the time of measurement (℃)</t>
+  </si>
+  <si>
+    <t>Solar radiation at the time of capture (W/m2)</t>
+  </si>
+  <si>
+    <t>Region (ventrum) * mass (g)</t>
+  </si>
+  <si>
+    <t>Region (head) * mass (g)</t>
+  </si>
+  <si>
+    <t>Region (dewlap) * mass (g)</t>
+  </si>
+  <si>
+    <t>Region (mite patch) * mass (g)</t>
+  </si>
+  <si>
+    <t>Region (ventrum) * temperature at the time of capture (℃)</t>
+  </si>
+  <si>
+    <t>Region (head) * temperature at the time of capture (℃)</t>
+  </si>
+  <si>
+    <t>Region (dewlap) * temperature at the time of capture (℃)</t>
+  </si>
+  <si>
+    <t>Region (mite patch) * temperature at the time of capture (℃)</t>
+  </si>
+  <si>
+    <t>Region (ventrum) * vapor pressure deficit at the time of capture (kPa)</t>
+  </si>
+  <si>
+    <t>Region (head) * vapor pressure deficit at the time of capture (kPa)</t>
+  </si>
+  <si>
+    <t>Region (dewlap) * vapor pressure deficit at the time of capture (kPa)</t>
+  </si>
+  <si>
+    <t>Region (mite patch) * vapor pressure deficit at the time of capture (kPa)</t>
+  </si>
+  <si>
+    <t>Wind (mph)</t>
+  </si>
+  <si>
+    <t>&lt; 0.05</t>
+  </si>
+  <si>
+    <t>&lt; 0.01</t>
+  </si>
+  <si>
+    <t>Body condition</t>
+  </si>
+  <si>
+    <t>Osmolality ~</t>
+  </si>
+  <si>
+    <t>Hematocrit ~</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -267,6 +280,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -613,15 +633,23 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -976,11 +1004,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37:D38"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1012,569 +1040,618 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
-        <v>-0.30855815155233701</v>
+        <v>-0.78162938545785898</v>
       </c>
       <c r="D3" s="1">
-        <v>0.65167615231006504</v>
+        <v>0.88173906861878204</v>
       </c>
       <c r="E3" s="1">
-        <v>-0.47348387762626898</v>
-      </c>
-      <c r="F3" s="1">
-        <v>417.69451130597901</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.63611536394532797</v>
+        <v>-0.88646336912603596</v>
+      </c>
+      <c r="F3" s="7">
+        <v>317.07269865839697</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.37603972745377301</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
-        <v>0.59031204411760896</v>
+        <v>0.85136101516218898</v>
       </c>
       <c r="D4" s="1">
-        <v>0.74674754704788904</v>
+        <v>0.90144809605607101</v>
       </c>
       <c r="E4" s="1">
-        <v>0.79051085798846499</v>
-      </c>
-      <c r="F4" s="1">
-        <v>489.97894053399898</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.42961191833200002</v>
+        <v>0.94443708837700402</v>
+      </c>
+      <c r="F4" s="7">
+        <v>489.62378410123603</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.34541213991511399</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1">
-        <v>0.268163233718338</v>
+        <v>0.42240715068533402</v>
       </c>
       <c r="D5" s="1">
-        <v>0.74888984372740297</v>
+        <v>0.90251399029236601</v>
       </c>
       <c r="E5" s="1">
-        <v>0.35808101280106203</v>
-      </c>
-      <c r="F5" s="1">
-        <v>490.674565725935</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.72043667922787902</v>
+        <v>0.46803390886882201</v>
+      </c>
+      <c r="F5" s="7">
+        <v>489.89145118163799</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.63996849275282996</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1">
-        <v>-2.0748167620985498</v>
+        <v>-1.7969918889708301</v>
       </c>
       <c r="D6" s="1">
-        <v>0.75501695566434202</v>
+        <v>0.90630023731884202</v>
       </c>
       <c r="E6" s="1">
-        <v>-2.74803995662973</v>
-      </c>
-      <c r="F6" s="1">
-        <v>492.76368984989898</v>
-      </c>
-      <c r="G6" s="3">
-        <v>6.2151144489930301E-3</v>
+        <v>-1.9827776877637899</v>
+      </c>
+      <c r="F6" s="7">
+        <v>491.00605774433001</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1">
-        <v>1.9844078770132501</v>
+        <v>2.5305313304218</v>
       </c>
       <c r="D7" s="1">
-        <v>0.75566313523664197</v>
+        <v>0.90733745847656599</v>
       </c>
       <c r="E7" s="1">
-        <v>2.6260482806162302</v>
-      </c>
-      <c r="F7" s="1">
-        <v>490.51153438827902</v>
-      </c>
-      <c r="G7" s="3">
-        <v>8.9082283460085593E-3</v>
+        <v>2.7889638047905501</v>
+      </c>
+      <c r="F7" s="7">
+        <v>489.92273658421902</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1">
-        <v>2.1104665875025901E-2</v>
+        <v>2.1099469259605E-2</v>
       </c>
       <c r="D8" s="1">
-        <v>1.3586417923446E-2</v>
+        <v>1.3581333132751601E-2</v>
       </c>
       <c r="E8" s="1">
-        <v>1.5533649850860101</v>
-      </c>
-      <c r="F8" s="1">
-        <v>466.01386126255102</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.121014797439165</v>
+        <v>1.5535639287665599</v>
+      </c>
+      <c r="F8" s="7">
+        <v>469.83590723510002</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.120961783402357</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1">
-        <v>-5.2415002628065803E-2</v>
+        <v>0.13595294388957799</v>
       </c>
       <c r="D9" s="1">
-        <v>1.4609722516875E-2</v>
+        <v>6.0622323140923598E-2</v>
       </c>
       <c r="E9" s="1">
-        <v>-3.5876795447363099</v>
-      </c>
-      <c r="F9" s="1">
-        <v>370.89749303831098</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>9</v>
+        <v>2.2426218073751398</v>
+      </c>
+      <c r="F9" s="7">
+        <v>347.70891829456099</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1">
-        <v>0.16279388095588801</v>
+        <v>-1.33618004613047</v>
       </c>
       <c r="D10" s="1">
-        <v>5.6786205766149102E-2</v>
+        <v>0.40462462349894202</v>
       </c>
       <c r="E10" s="1">
-        <v>2.8667856702081602</v>
-      </c>
-      <c r="F10" s="1">
-        <v>388.79172432175602</v>
+        <v>-3.30227071841554</v>
+      </c>
+      <c r="F10" s="7">
+        <v>384.31761336663197</v>
       </c>
       <c r="G10" s="3">
-        <v>4.3722408256069599E-3</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1">
-        <v>8.53840980396776E-2</v>
+        <v>8.2872883728317207E-2</v>
       </c>
       <c r="D11" s="1">
-        <v>1.36775756748116E-2</v>
+        <v>1.3348630295048699E-2</v>
       </c>
       <c r="E11" s="1">
-        <v>6.2426339337986398</v>
-      </c>
-      <c r="F11" s="1">
-        <v>121.842545650868</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>8</v>
+        <v>6.2083436200234496</v>
+      </c>
+      <c r="F11" s="7">
+        <v>120.63366999531399</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
-        <v>4.2447022183918101E-4</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1.7937266482454401E-4</v>
+        <v>19</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3.6762976385825298E-4</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.83941210752557E-4</v>
       </c>
       <c r="E12" s="1">
-        <v>2.3664153189360402</v>
-      </c>
-      <c r="F12" s="1">
-        <v>120.68674573873299</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1.9553314237877501E-2</v>
+        <v>1.99862642174732</v>
+      </c>
+      <c r="F12" s="7">
+        <v>119.954160414513</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1">
-        <v>2.4359907683766901E-2</v>
+        <v>-3.7593492778785501E-2</v>
       </c>
       <c r="D13" s="1">
-        <v>1.61431687550515E-2</v>
+        <v>5.4508948289226103E-2</v>
       </c>
       <c r="E13" s="1">
-        <v>1.50899170128196</v>
-      </c>
-      <c r="F13" s="1">
-        <v>493.77635206203797</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.13194048084552501</v>
+        <v>-0.68967562131841798</v>
+      </c>
+      <c r="F13" s="7">
+        <v>119.84782652906701</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.49173144329298502</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1">
-        <v>-1.6597053497131101E-2</v>
+        <v>2.4858216711060699E-2</v>
       </c>
       <c r="D14" s="1">
-        <v>1.6034718742493102E-2</v>
+        <v>1.6236838265568099E-2</v>
       </c>
       <c r="E14" s="1">
-        <v>-1.03506982340437</v>
-      </c>
-      <c r="F14" s="1">
-        <v>492.60955991782703</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0.30114415257892002</v>
+        <v>1.53097643177091</v>
+      </c>
+      <c r="F14" s="7">
+        <v>494.01846633780002</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.12641528905907901</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1">
-        <v>4.19922446074791E-2</v>
+        <v>-1.6443116911390901E-2</v>
       </c>
       <c r="D15" s="1">
-        <v>1.63949287850454E-2</v>
+        <v>1.61246159933791E-2</v>
       </c>
       <c r="E15" s="1">
-        <v>2.56129472460912</v>
-      </c>
-      <c r="F15" s="1">
-        <v>497.68629203155501</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1.07219272195962E-2</v>
+        <v>-1.01975246530786</v>
+      </c>
+      <c r="F15" s="7">
+        <v>492.76084161347097</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.30834626721054798</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1">
-        <v>4.3701636477455001E-2</v>
+        <v>4.1612076405109499E-2</v>
       </c>
       <c r="D16" s="1">
-        <v>1.6592095057942301E-2</v>
+        <v>1.6475114287298399E-2</v>
       </c>
       <c r="E16" s="1">
-        <v>2.6338829620275002</v>
-      </c>
-      <c r="F16" s="1">
-        <v>493.56091198321701</v>
-      </c>
-      <c r="G16" s="3">
-        <v>8.7064684269935501E-3</v>
+        <v>2.5257534290484802</v>
+      </c>
+      <c r="F16" s="7">
+        <v>497.76611515235402</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1.18542477115272E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1">
-        <v>4.42487313319751E-2</v>
+        <v>4.6107659910347099E-2</v>
       </c>
       <c r="D17" s="1">
-        <v>1.6136966795367799E-2</v>
+        <v>1.66713841652491E-2</v>
       </c>
       <c r="E17" s="1">
-        <v>2.7420724038842801</v>
-      </c>
-      <c r="F17" s="1">
-        <v>490.30545662283203</v>
-      </c>
-      <c r="G17" s="3">
-        <v>6.3285250570755402E-3</v>
+        <v>2.7656767700463001</v>
+      </c>
+      <c r="F17" s="7">
+        <v>493.72379615469401</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1">
-        <v>2.54967106846028E-2</v>
+        <v>-7.7216529803106906E-2</v>
       </c>
       <c r="D18" s="1">
-        <v>1.6128597528594298E-2</v>
+        <v>6.48277306311483E-2</v>
       </c>
       <c r="E18" s="1">
-        <v>1.58083867114917</v>
-      </c>
-      <c r="F18" s="1">
-        <v>490.590347072334</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0.114559404415277</v>
+        <v>-1.1911033912701201</v>
+      </c>
+      <c r="F18" s="7">
+        <v>489.27919329336299</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.234190493514286</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1">
-        <v>9.0254190275941296E-2</v>
+        <v>-1.33515660666457E-2</v>
       </c>
       <c r="D19" s="1">
-        <v>1.6148553632850001E-2</v>
+        <v>6.4837356030711293E-2</v>
       </c>
       <c r="E19" s="1">
-        <v>5.5889952950549597</v>
-      </c>
-      <c r="F19" s="1">
-        <v>491.05435680636202</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>8</v>
+        <v>-0.20592397475803201</v>
+      </c>
+      <c r="F19" s="7">
+        <v>489.34966819127698</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.83693593854140003</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1">
-        <v>6.3184628423583994E-2</v>
+        <v>5.71879415396747E-2</v>
       </c>
       <c r="D20" s="1">
-        <v>1.6042529131877901E-2</v>
+        <v>6.4945114449534797E-2</v>
       </c>
       <c r="E20" s="1">
-        <v>3.93857027805115</v>
-      </c>
-      <c r="F20" s="1">
-        <v>489.17352248805099</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>8</v>
+        <v>0.88055802232995195</v>
+      </c>
+      <c r="F20" s="7">
+        <v>489.92179783129097</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.37898883451704002</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1">
-        <v>-0.12678227142220799</v>
+        <v>-0.24522829002535301</v>
       </c>
       <c r="D21" s="1">
-        <v>6.33244826327687E-2</v>
+        <v>6.5003118115059003E-2</v>
       </c>
       <c r="E21" s="1">
-        <v>-2.00210512823995</v>
-      </c>
-      <c r="F21" s="1">
-        <v>489.47799328830502</v>
-      </c>
-      <c r="G21" s="3">
-        <v>4.5824664055568898E-2</v>
+        <v>-3.7725619498942402</v>
+      </c>
+      <c r="F21" s="7">
+        <v>489.45349023857801</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="1">
-        <v>-3.38737399273559E-2</v>
+        <v>0.85992271797952602</v>
       </c>
       <c r="D22" s="1">
-        <v>6.3338381628292806E-2</v>
+        <v>0.45100164503008899</v>
       </c>
       <c r="E22" s="1">
-        <v>-0.534805895833385</v>
-      </c>
-      <c r="F22" s="1">
-        <v>489.56565243299099</v>
-      </c>
-      <c r="G22" s="3">
-        <v>0.59302689329597102</v>
+        <v>1.9066953024576101</v>
+      </c>
+      <c r="F22" s="7">
+        <v>489.31764797780801</v>
+      </c>
+      <c r="G22" s="5">
+        <v>5.7145479618461899E-2</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="1">
-        <v>-1.54089399575882E-2</v>
+        <v>0.27436741364480399</v>
       </c>
       <c r="D23" s="1">
-        <v>6.3715637688670307E-2</v>
+        <v>0.45100041967744597</v>
       </c>
       <c r="E23" s="1">
-        <v>-0.24183921744423201</v>
-      </c>
-      <c r="F23" s="1">
-        <v>491.458032032983</v>
-      </c>
-      <c r="G23" s="3">
-        <v>0.80900562602619297</v>
+        <v>0.60835290095967198</v>
+      </c>
+      <c r="F23" s="7">
+        <v>489.31550373505701</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.543235721518736</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.23521869797085801</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.45213468437452797</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.52024033125495195</v>
+      </c>
+      <c r="F24" s="7">
+        <v>490.19785752067901</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.60313094843038995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="1">
-        <v>-0.331890158924459</v>
-      </c>
-      <c r="D24" s="1">
-        <v>6.3981420002780801E-2</v>
-      </c>
-      <c r="E24" s="1">
-        <v>-5.1872896680010303</v>
-      </c>
-      <c r="F24" s="1">
-        <v>490.20556949830802</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="C25" s="1">
+        <v>2.1796292688328198</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.45313583510703098</v>
+      </c>
+      <c r="E25" s="1">
+        <v>4.8101012984726603</v>
+      </c>
+      <c r="F25" s="7">
+        <v>489.65446102133001</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26">
-        <v>861.25</v>
-      </c>
-      <c r="D26">
-        <v>330.66</v>
-      </c>
-      <c r="E26">
-        <v>2.61</v>
-      </c>
-      <c r="F26">
-        <v>20.28</v>
-      </c>
-      <c r="G26" s="2">
-        <v>1.7000000000000001E-2</v>
-      </c>
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27">
-        <v>-57.9</v>
-      </c>
-      <c r="D27">
-        <v>36.76</v>
-      </c>
-      <c r="E27">
-        <v>-1.58</v>
-      </c>
-      <c r="F27">
-        <v>13.21</v>
-      </c>
-      <c r="G27" s="2">
-        <v>0.13900000000000001</v>
+        <v>9</v>
+      </c>
+      <c r="C27" s="1">
+        <v>288.68177536175801</v>
+      </c>
+      <c r="D27" s="1">
+        <v>119.095703958078</v>
+      </c>
+      <c r="E27" s="1">
+        <v>2.42394784839068</v>
+      </c>
+      <c r="F27" s="7">
+        <v>18.7787602828388</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28">
-        <v>-28.06</v>
-      </c>
-      <c r="D28">
-        <v>17.78</v>
-      </c>
-      <c r="E28">
-        <v>-1.58</v>
-      </c>
-      <c r="F28">
-        <v>17.71</v>
-      </c>
-      <c r="G28" s="2">
-        <v>0.13200000000000001</v>
+        <v>12</v>
+      </c>
+      <c r="C28" s="1">
+        <v>142.80297498702501</v>
+      </c>
+      <c r="D28" s="1">
+        <v>248.35750289810699</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.57498957478893697</v>
+      </c>
+      <c r="F28" s="7">
+        <v>8.8915191725453901</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.579554580618174</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29">
-        <v>3.25</v>
-      </c>
-      <c r="D29">
-        <v>1.97</v>
-      </c>
-      <c r="E29">
-        <v>1.65</v>
-      </c>
-      <c r="F29">
-        <v>11.89</v>
-      </c>
-      <c r="G29" s="2">
-        <v>0.126</v>
+        <v>11</v>
+      </c>
+      <c r="C29" s="1">
+        <v>3.5783445681338399</v>
+      </c>
+      <c r="D29" s="1">
+        <v>5.9177931101782102</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.60467551019641497</v>
+      </c>
+      <c r="F29" s="7">
+        <v>53.260214273555803</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0.54796218137789299</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>7</v>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="1">
+        <v>-0.869154839540766</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1.2506411079259201</v>
+      </c>
+      <c r="E30" s="1">
+        <v>-0.69496743232931402</v>
+      </c>
+      <c r="F30" s="7">
+        <v>112.519089359452</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.48850837505129602</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1">
+        <v>-5.8005524728102298</v>
+      </c>
+      <c r="D31" s="1">
+        <v>9.5158483746553202</v>
+      </c>
+      <c r="E31" s="1">
+        <v>-0.60956755976267096</v>
+      </c>
+      <c r="F31" s="7">
+        <v>9.4498422827578192</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.55651948054165101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33">
         <v>33.659999999999997</v>
       </c>
-      <c r="D31">
+      <c r="D33">
         <v>0.88</v>
       </c>
-      <c r="E31">
+      <c r="E33">
         <v>38.409999999999997</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="F33" s="7">
+        <v>117</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+      <c r="C34">
+        <v>2.67</v>
+      </c>
+      <c r="D34">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E34">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="F34" s="7">
+        <v>119</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C32">
-        <v>2.67</v>
-      </c>
-      <c r="D32">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E32">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="F32">
-        <v>119</v>
-      </c>
-      <c r="G32" s="2">
-        <v>1.7000000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>